<commit_message>
adding different dividend summary api
</commit_message>
<xml_diff>
--- a/portfolio-manager/src/main/resources/mydata/invested.xlsx
+++ b/portfolio-manager/src/main/resources/mydata/invested.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\hp-pendrive\documents\my-documents\FINANCE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\hp-pendrive\documents\my-documents\FINANCE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D9C6FC6-2E98-47C0-A581-7D88E263EFD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5B44ADF-EC06-4ECE-AFF9-68F3BB61D040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="life-goal-timeline" sheetId="6" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">dividend!$B$1:$H$115</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">dividend!$B$1:$H$116</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="256">
   <si>
     <t>sbi</t>
   </si>
@@ -677,6 +677,138 @@
   </si>
   <si>
     <t>JBCHEPHARM</t>
+  </si>
+  <si>
+    <t>MOTHERSON</t>
+  </si>
+  <si>
+    <t>Samvardhana Motherson International Limited</t>
+  </si>
+  <si>
+    <t>WIPRO</t>
+  </si>
+  <si>
+    <t>Wipro Limited</t>
+  </si>
+  <si>
+    <t>VEDL</t>
+  </si>
+  <si>
+    <t>Vedanta Limited</t>
+  </si>
+  <si>
+    <t>TRIDENT</t>
+  </si>
+  <si>
+    <t>Trident Limited</t>
+  </si>
+  <si>
+    <t>TCS</t>
+  </si>
+  <si>
+    <t>Tata Consultancy Services Limited</t>
+  </si>
+  <si>
+    <t>TPLPLASTEH</t>
+  </si>
+  <si>
+    <t>TPL Plastech Limited</t>
+  </si>
+  <si>
+    <t>TATA Steel Limited</t>
+  </si>
+  <si>
+    <t>TATASTEEL</t>
+  </si>
+  <si>
+    <t>TATAPOWER</t>
+  </si>
+  <si>
+    <t>Tata Power Company Limited</t>
+  </si>
+  <si>
+    <t>TATACHEM</t>
+  </si>
+  <si>
+    <t>Tata Chemicals Limited</t>
+  </si>
+  <si>
+    <t>STLTECH</t>
+  </si>
+  <si>
+    <t>Sterlite Technologies Limited</t>
+  </si>
+  <si>
+    <t>SBILIFE</t>
+  </si>
+  <si>
+    <t>SBI Life Insurance Company Limited</t>
+  </si>
+  <si>
+    <t>SBICARD</t>
+  </si>
+  <si>
+    <t>SBI Cards and Payment Services Limited</t>
+  </si>
+  <si>
+    <t>SBIN</t>
+  </si>
+  <si>
+    <t>State Bank of India</t>
+  </si>
+  <si>
+    <t>ROUTE</t>
+  </si>
+  <si>
+    <t>ROUTE MOBILE LIMITED</t>
+  </si>
+  <si>
+    <t>RELIANCE</t>
+  </si>
+  <si>
+    <t>Reliance Industries Limited</t>
+  </si>
+  <si>
+    <t>PRINCEPIPE</t>
+  </si>
+  <si>
+    <t>Prince Pipes And Fittings Limited</t>
+  </si>
+  <si>
+    <t>PRAJIND</t>
+  </si>
+  <si>
+    <t>Praj Industries Limited</t>
+  </si>
+  <si>
+    <t>PIIND</t>
+  </si>
+  <si>
+    <t>PI Industries Limited</t>
+  </si>
+  <si>
+    <t>PIDILITIND</t>
+  </si>
+  <si>
+    <t>Pidilite Industries Limited</t>
+  </si>
+  <si>
+    <t>NESTLEIND</t>
+  </si>
+  <si>
+    <t>Nestle India Limited</t>
+  </si>
+  <si>
+    <t>LAURUSLABS</t>
+  </si>
+  <si>
+    <t>Laurus Labs Limited</t>
+  </si>
+  <si>
+    <t>KEC</t>
+  </si>
+  <si>
+    <t>KEC International Limited</t>
   </si>
 </sst>
 </file>
@@ -809,7 +941,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -841,9 +973,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1282,10 +1411,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85F45F4A-D0C5-4A27-95D9-03BBBD885C19}">
-  <dimension ref="A1:R115"/>
+  <dimension ref="A1:R116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="E84" sqref="E84"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1294,7 +1423,7 @@
     <col min="2" max="2" width="7.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="40" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
@@ -1363,8 +1492,12 @@
       <c r="C3" s="2">
         <v>1</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>233</v>
+      </c>
       <c r="F3" s="2" t="s">
         <v>32</v>
       </c>
@@ -1382,8 +1515,12 @@
       <c r="C4" s="2">
         <v>1</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>251</v>
+      </c>
       <c r="F4" s="2" t="s">
         <v>56</v>
       </c>
@@ -1447,8 +1584,12 @@
       <c r="C7" s="2">
         <v>1</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>221</v>
+      </c>
       <c r="F7" s="2" t="s">
         <v>39</v>
       </c>
@@ -1466,8 +1607,12 @@
       <c r="C8" s="2">
         <v>1</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>237</v>
+      </c>
       <c r="F8" s="2" t="s">
         <v>0</v>
       </c>
@@ -1508,8 +1653,12 @@
       <c r="C10" s="2">
         <v>1</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>241</v>
+      </c>
       <c r="F10" s="2" t="s">
         <v>64</v>
       </c>
@@ -1550,8 +1699,12 @@
       <c r="C12" s="2">
         <v>1</v>
       </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="D12" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>223</v>
+      </c>
       <c r="F12" s="2" t="s">
         <v>65</v>
       </c>
@@ -1619,8 +1772,12 @@
       <c r="C15" s="3">
         <v>2</v>
       </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
+      <c r="D15" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>229</v>
+      </c>
       <c r="F15" s="3" t="s">
         <v>68</v>
       </c>
@@ -1638,8 +1795,12 @@
       <c r="C16" s="3">
         <v>2</v>
       </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
+      <c r="D16" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>227</v>
+      </c>
       <c r="F16" s="3" t="s">
         <v>67</v>
       </c>
@@ -1795,8 +1956,12 @@
       <c r="C23" s="3">
         <v>2</v>
       </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
+      <c r="D23" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>221</v>
+      </c>
       <c r="F23" s="3" t="s">
         <v>39</v>
       </c>
@@ -1906,8 +2071,12 @@
       <c r="C28" s="3">
         <v>2</v>
       </c>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
+      <c r="D28" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>239</v>
+      </c>
       <c r="F28" s="3" t="s">
         <v>43</v>
       </c>
@@ -1925,8 +2094,12 @@
       <c r="C29" s="3">
         <v>2</v>
       </c>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
+      <c r="D29" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>255</v>
+      </c>
       <c r="F29" s="3" t="s">
         <v>76</v>
       </c>
@@ -1990,8 +2163,12 @@
       <c r="C32" s="3">
         <v>2</v>
       </c>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
+      <c r="D32" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>249</v>
+      </c>
       <c r="F32" s="3" t="s">
         <v>78</v>
       </c>
@@ -2147,8 +2324,12 @@
       <c r="C39" s="3">
         <v>2</v>
       </c>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
+      <c r="D39" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>245</v>
+      </c>
       <c r="F39" s="3" t="s">
         <v>80</v>
       </c>
@@ -2212,8 +2393,12 @@
       <c r="C42" s="3">
         <v>2</v>
       </c>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
+      <c r="D42" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>231</v>
+      </c>
       <c r="F42" s="3" t="s">
         <v>83</v>
       </c>
@@ -2367,8 +2552,12 @@
       <c r="C49" s="3">
         <v>2</v>
       </c>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
+      <c r="D49" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>243</v>
+      </c>
       <c r="F49" s="3" t="s">
         <v>59</v>
       </c>
@@ -2409,8 +2598,12 @@
       <c r="C51" s="3">
         <v>2</v>
       </c>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
+      <c r="D51" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>213</v>
+      </c>
       <c r="F51" s="3" t="s">
         <v>88</v>
       </c>
@@ -2478,8 +2671,12 @@
       <c r="C54" s="4">
         <v>3</v>
       </c>
-      <c r="D54" s="4"/>
-      <c r="E54" s="4"/>
+      <c r="D54" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>247</v>
+      </c>
       <c r="F54" s="4" t="s">
         <v>46</v>
       </c>
@@ -2543,8 +2740,12 @@
       <c r="C57" s="4">
         <v>3</v>
       </c>
-      <c r="D57" s="4"/>
-      <c r="E57" s="4"/>
+      <c r="D57" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>221</v>
+      </c>
       <c r="F57" s="4" t="s">
         <v>39</v>
       </c>
@@ -2631,8 +2832,12 @@
       <c r="C61" s="4">
         <v>3</v>
       </c>
-      <c r="D61" s="4"/>
-      <c r="E61" s="4"/>
+      <c r="D61" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>219</v>
+      </c>
       <c r="F61" s="4" t="s">
         <v>55</v>
       </c>
@@ -2650,8 +2855,12 @@
       <c r="C62" s="4">
         <v>3</v>
       </c>
-      <c r="D62" s="4"/>
-      <c r="E62" s="4"/>
+      <c r="D62" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>251</v>
+      </c>
       <c r="F62" s="4" t="s">
         <v>56</v>
       </c>
@@ -2761,8 +2970,12 @@
       <c r="C67" s="4">
         <v>3</v>
       </c>
-      <c r="D67" s="4"/>
-      <c r="E67" s="4"/>
+      <c r="D67" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>243</v>
+      </c>
       <c r="F67" s="4" t="s">
         <v>59</v>
       </c>
@@ -2780,8 +2993,12 @@
       <c r="C68" s="4">
         <v>3</v>
       </c>
-      <c r="D68" s="4"/>
-      <c r="E68" s="4"/>
+      <c r="D68" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>253</v>
+      </c>
       <c r="F68" s="4" t="s">
         <v>35</v>
       </c>
@@ -2918,8 +3135,12 @@
       <c r="C74" s="5">
         <v>4</v>
       </c>
-      <c r="D74" s="5"/>
-      <c r="E74" s="5"/>
+      <c r="D74" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="E74" s="5" t="s">
+        <v>215</v>
+      </c>
       <c r="F74" s="5" t="s">
         <v>33</v>
       </c>
@@ -2960,8 +3181,12 @@
       <c r="C76" s="5">
         <v>4</v>
       </c>
-      <c r="D76" s="5"/>
-      <c r="E76" s="5"/>
+      <c r="D76" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>221</v>
+      </c>
       <c r="F76" s="5" t="s">
         <v>39</v>
       </c>
@@ -3048,8 +3273,12 @@
       <c r="C80" s="5">
         <v>4</v>
       </c>
-      <c r="D80" s="5"/>
-      <c r="E80" s="5"/>
+      <c r="D80" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="E80" s="5" t="s">
+        <v>239</v>
+      </c>
       <c r="F80" s="5" t="s">
         <v>43</v>
       </c>
@@ -3113,8 +3342,12 @@
       <c r="C83" s="5">
         <v>4</v>
       </c>
-      <c r="D83" s="5"/>
-      <c r="E83" s="5"/>
+      <c r="D83" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="E83" s="5" t="s">
+        <v>247</v>
+      </c>
       <c r="F83" s="5" t="s">
         <v>46</v>
       </c>
@@ -3201,8 +3434,12 @@
       <c r="C87" s="5">
         <v>4</v>
       </c>
-      <c r="D87" s="5"/>
-      <c r="E87" s="5"/>
+      <c r="D87" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E87" s="5" t="s">
+        <v>217</v>
+      </c>
       <c r="F87" s="5" t="s">
         <v>36</v>
       </c>
@@ -3224,8 +3461,12 @@
       <c r="C88" s="2">
         <v>1</v>
       </c>
-      <c r="D88" s="2"/>
-      <c r="E88" s="2"/>
+      <c r="D88" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>235</v>
+      </c>
       <c r="F88" s="2" t="s">
         <v>31</v>
       </c>
@@ -3243,8 +3484,12 @@
       <c r="C89" s="2">
         <v>1</v>
       </c>
-      <c r="D89" s="2"/>
-      <c r="E89" s="2"/>
+      <c r="D89" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>233</v>
+      </c>
       <c r="F89" s="2" t="s">
         <v>32</v>
       </c>
@@ -3262,8 +3507,12 @@
       <c r="C90" s="2">
         <v>1</v>
       </c>
-      <c r="D90" s="2"/>
-      <c r="E90" s="2"/>
+      <c r="D90" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>215</v>
+      </c>
       <c r="F90" s="2" t="s">
         <v>33</v>
       </c>
@@ -3304,8 +3553,12 @@
       <c r="C92" s="2">
         <v>1</v>
       </c>
-      <c r="D92" s="2"/>
-      <c r="E92" s="2"/>
+      <c r="D92" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>253</v>
+      </c>
       <c r="F92" s="2" t="s">
         <v>35</v>
       </c>
@@ -3323,8 +3576,12 @@
       <c r="C93" s="2">
         <v>1</v>
       </c>
-      <c r="D93" s="2"/>
-      <c r="E93" s="2"/>
+      <c r="D93" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>217</v>
+      </c>
       <c r="F93" s="2" t="s">
         <v>36</v>
       </c>
@@ -3392,8 +3649,12 @@
       <c r="C96" s="3">
         <v>2</v>
       </c>
-      <c r="D96" s="3"/>
-      <c r="E96" s="3"/>
+      <c r="D96" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="E96" s="3" t="s">
+        <v>224</v>
+      </c>
       <c r="F96" s="3" t="s">
         <v>122</v>
       </c>
@@ -3465,8 +3726,12 @@
       <c r="C99" s="3">
         <v>2</v>
       </c>
-      <c r="D99" s="3"/>
-      <c r="E99" s="3"/>
+      <c r="D99" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="E99" s="3" t="s">
+        <v>229</v>
+      </c>
       <c r="F99" s="3" t="s">
         <v>68</v>
       </c>
@@ -3488,8 +3753,12 @@
       <c r="C100" s="3">
         <v>2</v>
       </c>
-      <c r="D100" s="3"/>
-      <c r="E100" s="3"/>
+      <c r="D100" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="E100" s="3" t="s">
+        <v>227</v>
+      </c>
       <c r="F100" s="3" t="s">
         <v>67</v>
       </c>
@@ -3511,8 +3780,12 @@
       <c r="C101" s="3">
         <v>2</v>
       </c>
-      <c r="D101" s="3"/>
-      <c r="E101" s="3"/>
+      <c r="D101" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="E101" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="F101" s="3" t="s">
         <v>75</v>
       </c>
@@ -3615,8 +3888,12 @@
       <c r="C105" s="3">
         <v>2</v>
       </c>
-      <c r="D105" s="3"/>
-      <c r="E105" s="3"/>
+      <c r="D105" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E105" s="3" t="s">
+        <v>221</v>
+      </c>
       <c r="F105" s="3" t="s">
         <v>39</v>
       </c>
@@ -3638,8 +3915,12 @@
       <c r="C106" s="3">
         <v>2</v>
       </c>
-      <c r="D106" s="3"/>
-      <c r="E106" s="3"/>
+      <c r="D106" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="E106" s="3" t="s">
+        <v>217</v>
+      </c>
       <c r="F106" s="3" t="s">
         <v>36</v>
       </c>
@@ -3827,8 +4108,12 @@
       <c r="C113" s="3">
         <v>2</v>
       </c>
-      <c r="D113" s="3"/>
-      <c r="E113" s="3"/>
+      <c r="D113" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="E113" s="3" t="s">
+        <v>245</v>
+      </c>
       <c r="F113" s="3" t="s">
         <v>80</v>
       </c>
@@ -3861,19 +4146,15 @@
       <c r="G114" s="3">
         <v>120</v>
       </c>
-      <c r="H114" s="1">
-        <f>SUM(G95:G114)</f>
-        <v>3699.25</v>
-      </c>
       <c r="I114" s="1" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A115" s="1">
+      <c r="A115" s="3">
         <v>114</v>
       </c>
-      <c r="B115" s="1">
+      <c r="B115" s="3">
         <v>2022</v>
       </c>
       <c r="C115" s="3">
@@ -3882,18 +4163,41 @@
       <c r="D115" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="E115" s="14" t="s">
+      <c r="E115" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="F115" s="1" t="s">
+      <c r="F115" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="G115" s="1">
+      <c r="G115" s="3">
         <v>306</v>
       </c>
     </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A116" s="3">
+        <v>115</v>
+      </c>
+      <c r="B116" s="3">
+        <v>2022</v>
+      </c>
+      <c r="C116" s="3">
+        <v>2</v>
+      </c>
+      <c r="D116" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="E116" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="F116" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G116" s="3">
+        <v>156</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="B1:H115" xr:uid="{85F45F4A-D0C5-4A27-95D9-03BBBD885C19}"/>
+  <autoFilter ref="B1:H116" xr:uid="{85F45F4A-D0C5-4A27-95D9-03BBBD885C19}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3958,7 +4262,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="12" t="s">
@@ -3999,7 +4303,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
+      <c r="A3" s="14"/>
       <c r="B3" s="12" t="s">
         <v>7</v>
       </c>
@@ -4038,7 +4342,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
+      <c r="A4" s="14"/>
       <c r="B4" s="12" t="s">
         <v>8</v>
       </c>
@@ -4073,7 +4377,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
+      <c r="A5" s="14"/>
       <c r="B5" s="12" t="s">
         <v>2</v>
       </c>
@@ -4112,7 +4416,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
+      <c r="A6" s="14"/>
       <c r="B6" s="12" t="s">
         <v>9</v>
       </c>
@@ -4143,7 +4447,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
+      <c r="A7" s="14"/>
       <c r="B7" s="12" t="s">
         <v>10</v>
       </c>
@@ -4182,7 +4486,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
+      <c r="A8" s="14"/>
       <c r="B8" s="12" t="s">
         <v>11</v>
       </c>
@@ -4211,7 +4515,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
+      <c r="A9" s="14"/>
       <c r="B9" s="12" t="s">
         <v>3</v>
       </c>
@@ -4250,7 +4554,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
+      <c r="A10" s="14"/>
       <c r="B10" s="12" t="s">
         <v>13</v>
       </c>
@@ -4287,7 +4591,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
+      <c r="A11" s="14"/>
       <c r="B11" s="12" t="s">
         <v>16</v>
       </c>
@@ -4320,7 +4624,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
+      <c r="A12" s="14"/>
       <c r="B12" s="12" t="s">
         <v>21</v>
       </c>
@@ -4347,7 +4651,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
+      <c r="A13" s="14"/>
       <c r="B13" s="12" t="s">
         <v>25</v>
       </c>
@@ -4372,7 +4676,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
+      <c r="A14" s="14"/>
       <c r="B14" s="12" t="s">
         <v>24</v>
       </c>
@@ -4395,7 +4699,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
+      <c r="A15" s="14"/>
       <c r="B15" s="12" t="s">
         <v>126</v>
       </c>
@@ -4418,7 +4722,7 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="15"/>
+      <c r="A16" s="14"/>
       <c r="B16" s="12"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
@@ -4433,7 +4737,7 @@
       <c r="M16" s="8"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
+      <c r="A17" s="14"/>
       <c r="B17" s="12"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
@@ -4448,7 +4752,7 @@
       <c r="M17" s="8"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
+      <c r="A18" s="14"/>
       <c r="B18" s="12" t="s">
         <v>0</v>
       </c>
@@ -4479,7 +4783,7 @@
       <c r="M18" s="8"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
+      <c r="A19" s="14"/>
       <c r="B19" s="12" t="s">
         <v>12</v>
       </c>
@@ -4510,7 +4814,7 @@
       <c r="M19" s="8"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="15"/>
+      <c r="A20" s="14"/>
       <c r="B20" s="12" t="s">
         <v>1</v>
       </c>
@@ -4541,7 +4845,7 @@
       <c r="M20" s="8"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="15"/>
+      <c r="A21" s="14"/>
       <c r="B21" s="12"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
@@ -4556,7 +4860,7 @@
       <c r="M21" s="8"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="15"/>
+      <c r="A22" s="14"/>
       <c r="B22" s="12"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
@@ -4571,7 +4875,7 @@
       <c r="M22" s="8"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="15"/>
+      <c r="A23" s="14"/>
       <c r="B23" s="12" t="s">
         <v>22</v>
       </c>
@@ -4596,10 +4900,10 @@
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="16" t="s">
+      <c r="A27" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="B27" s="17"/>
+      <c r="B27" s="16"/>
       <c r="C27" s="10"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
adding more dividend api
</commit_message>
<xml_diff>
--- a/portfolio-manager/src/main/resources/mydata/invested.xlsx
+++ b/portfolio-manager/src/main/resources/mydata/invested.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\hp-pendrive\documents\my-documents\FINANCE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\hp-pendrive\documents\my-documents\FINANCE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5B44ADF-EC06-4ECE-AFF9-68F3BB61D040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA004366-37BA-49C3-A692-70667DACAA00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="256">
   <si>
     <t>sbi</t>
   </si>
@@ -1413,8 +1413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85F45F4A-D0C5-4A27-95D9-03BBBD885C19}">
   <dimension ref="A1:R116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2488,7 +2488,9 @@
       <c r="D46" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="E46" s="3"/>
+      <c r="E46" s="3" t="s">
+        <v>138</v>
+      </c>
       <c r="F46" s="3" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
changes in portfolio-manger background
</commit_message>
<xml_diff>
--- a/portfolio-manager/src/main/resources/mydata/invested.xlsx
+++ b/portfolio-manager/src/main/resources/mydata/invested.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\hp-pendrive\documents\my-documents\FINANCE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA004366-37BA-49C3-A692-70667DACAA00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{433457A5-9222-4EEB-BD7B-68465041AAB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="255">
   <si>
     <t>sbi</t>
   </si>
@@ -58,9 +58,6 @@
     <t>date</t>
   </si>
   <si>
-    <t>asset class</t>
-  </si>
-  <si>
     <t>zerodha kite</t>
   </si>
   <si>
@@ -418,9 +415,6 @@
     <t>amaraRajaBatteries</t>
   </si>
   <si>
-    <t>not credit yet</t>
-  </si>
-  <si>
     <t>lic</t>
   </si>
   <si>
@@ -809,6 +803,9 @@
   </si>
   <si>
     <t>KEC International Limited</t>
+  </si>
+  <si>
+    <t>17th aug</t>
   </si>
 </sst>
 </file>
@@ -888,7 +885,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -937,11 +934,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -974,9 +982,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1278,16 +1285,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>91</v>
-      </c>
       <c r="D1" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1295,13 +1302,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C2" s="7">
         <v>9000</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1309,13 +1316,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C3" s="7">
         <v>3000</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1323,13 +1330,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C4" s="7">
         <v>14000</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1337,13 +1344,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C5" s="7">
         <v>2500</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1351,13 +1358,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C6" s="7">
         <v>15000</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1365,13 +1372,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C7" s="7">
         <v>6500</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1400,7 +1407,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1411,10 +1418,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85F45F4A-D0C5-4A27-95D9-03BBBD885C19}">
-  <dimension ref="A1:R116"/>
+  <dimension ref="A1:R122"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="D124" sqref="D124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1435,28 +1442,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1470,13 +1477,13 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G2" s="2">
         <v>186</v>
@@ -1493,13 +1500,13 @@
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G3" s="2">
         <v>22</v>
@@ -1516,13 +1523,13 @@
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G4" s="2">
         <v>90</v>
@@ -1539,13 +1546,13 @@
         <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G5" s="2">
         <v>52</v>
@@ -1562,13 +1569,13 @@
         <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G6" s="2">
         <v>37</v>
@@ -1585,13 +1592,13 @@
         <v>1</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G7" s="2">
         <v>15</v>
@@ -1608,10 +1615,10 @@
         <v>1</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>0</v>
@@ -1631,13 +1638,13 @@
         <v>1</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G9" s="2">
         <v>34</v>
@@ -1654,13 +1661,13 @@
         <v>1</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G10" s="2">
         <v>70</v>
@@ -1677,13 +1684,13 @@
         <v>1</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G11" s="2">
         <v>210</v>
@@ -1700,13 +1707,13 @@
         <v>1</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G12" s="2">
         <v>50</v>
@@ -1727,13 +1734,13 @@
         <v>2</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G13" s="3">
         <v>29</v>
@@ -1750,13 +1757,13 @@
         <v>2</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G14" s="3">
         <v>8</v>
@@ -1773,13 +1780,13 @@
         <v>2</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G15" s="3">
         <v>200</v>
@@ -1796,13 +1803,13 @@
         <v>2</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G16" s="3">
         <v>147</v>
@@ -1819,13 +1826,13 @@
         <v>2</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G17" s="3">
         <v>36</v>
@@ -1842,13 +1849,13 @@
         <v>2</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G18" s="3">
         <v>68</v>
@@ -1865,13 +1872,13 @@
         <v>2</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G19" s="3">
         <v>12</v>
@@ -1888,13 +1895,13 @@
         <v>2</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G20" s="3">
         <v>50</v>
@@ -1911,13 +1918,13 @@
         <v>2</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G21" s="3">
         <v>48</v>
@@ -1934,13 +1941,13 @@
         <v>2</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G22" s="3">
         <v>50</v>
@@ -1957,13 +1964,13 @@
         <v>2</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G23" s="3">
         <v>14</v>
@@ -1980,13 +1987,13 @@
         <v>2</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G24" s="3">
         <v>88</v>
@@ -2003,13 +2010,13 @@
         <v>2</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G25" s="3">
         <v>13</v>
@@ -2026,13 +2033,13 @@
         <v>2</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G26" s="3">
         <v>140</v>
@@ -2049,13 +2056,13 @@
         <v>2</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G27" s="3">
         <v>35</v>
@@ -2072,13 +2079,13 @@
         <v>2</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G28" s="3">
         <v>12</v>
@@ -2095,13 +2102,13 @@
         <v>2</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G29" s="3">
         <v>12</v>
@@ -2118,13 +2125,13 @@
         <v>2</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G30" s="3">
         <v>48</v>
@@ -2141,13 +2148,13 @@
         <v>2</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G31" s="3">
         <v>19</v>
@@ -2164,13 +2171,13 @@
         <v>2</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G32" s="3">
         <v>34</v>
@@ -2187,13 +2194,13 @@
         <v>2</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G33" s="3">
         <v>368</v>
@@ -2210,13 +2217,13 @@
         <v>2</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G34" s="3">
         <v>4</v>
@@ -2233,13 +2240,13 @@
         <v>2</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G35" s="3">
         <v>6</v>
@@ -2256,13 +2263,13 @@
         <v>2</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G36" s="3">
         <v>78</v>
@@ -2279,13 +2286,13 @@
         <v>2</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G37" s="3">
         <v>8</v>
@@ -2302,13 +2309,13 @@
         <v>2</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G38" s="3">
         <v>50</v>
@@ -2325,13 +2332,13 @@
         <v>2</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G39" s="3">
         <v>19</v>
@@ -2348,13 +2355,13 @@
         <v>2</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G40" s="3">
         <v>60</v>
@@ -2371,13 +2378,13 @@
         <v>2</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G41" s="3">
         <v>40</v>
@@ -2394,13 +2401,13 @@
         <v>2</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G42" s="3">
         <v>40</v>
@@ -2417,13 +2424,13 @@
         <v>2</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G43" s="3">
         <v>2</v>
@@ -2440,13 +2447,13 @@
         <v>2</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G44" s="3">
         <v>15</v>
@@ -2463,13 +2470,13 @@
         <v>2</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G45" s="3">
         <v>33</v>
@@ -2486,13 +2493,13 @@
         <v>2</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G46" s="3">
         <v>4</v>
@@ -2509,13 +2516,13 @@
         <v>2</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G47" s="3">
         <v>165</v>
@@ -2532,13 +2539,13 @@
         <v>2</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G48" s="3">
         <v>24</v>
@@ -2555,13 +2562,13 @@
         <v>2</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G49" s="3">
         <v>18</v>
@@ -2578,13 +2585,13 @@
         <v>2</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G50" s="3">
         <v>40</v>
@@ -2601,13 +2608,13 @@
         <v>2</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G51" s="3">
         <v>240</v>
@@ -2624,13 +2631,13 @@
         <v>2</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G52" s="3">
         <v>10</v>
@@ -2647,13 +2654,13 @@
         <v>2</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G53" s="3">
         <v>12</v>
@@ -2674,13 +2681,13 @@
         <v>3</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G54" s="4">
         <v>4</v>
@@ -2697,13 +2704,13 @@
         <v>3</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G55" s="4">
         <v>52</v>
@@ -2720,13 +2727,13 @@
         <v>3</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G56" s="4">
         <v>9</v>
@@ -2743,13 +2750,13 @@
         <v>3</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G57" s="4">
         <v>20</v>
@@ -2766,13 +2773,13 @@
         <v>3</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G58" s="4">
         <v>1240</v>
@@ -2789,13 +2796,13 @@
         <v>3</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G59" s="4">
         <v>480</v>
@@ -2812,13 +2819,13 @@
         <v>3</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G60" s="4">
         <v>30</v>
@@ -2835,13 +2842,13 @@
         <v>3</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G61" s="4">
         <v>18</v>
@@ -2858,13 +2865,13 @@
         <v>3</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G62" s="4">
         <v>110</v>
@@ -2881,13 +2888,13 @@
         <v>3</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G63" s="4">
         <v>141</v>
@@ -2904,13 +2911,13 @@
         <v>3</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G64" s="4">
         <v>40</v>
@@ -2927,13 +2934,13 @@
         <v>3</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G65" s="4">
         <v>104</v>
@@ -2950,13 +2957,13 @@
         <v>3</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G66" s="4">
         <v>2</v>
@@ -2973,13 +2980,13 @@
         <v>3</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G67" s="4">
         <v>15</v>
@@ -2996,13 +3003,13 @@
         <v>3</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G68" s="4">
         <v>24</v>
@@ -3019,13 +3026,13 @@
         <v>3</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G69" s="4">
         <v>12</v>
@@ -3042,13 +3049,13 @@
         <v>3</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G70" s="4">
         <v>105</v>
@@ -3065,13 +3072,13 @@
         <v>3</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G71" s="4">
         <v>7</v>
@@ -3088,13 +3095,13 @@
         <v>3</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G72" s="4">
         <v>6</v>
@@ -3115,13 +3122,13 @@
         <v>4</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G73" s="5">
         <v>32</v>
@@ -3138,13 +3145,13 @@
         <v>4</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G74" s="5">
         <v>15</v>
@@ -3161,13 +3168,13 @@
         <v>4</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G75" s="5">
         <v>300</v>
@@ -3184,13 +3191,13 @@
         <v>4</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E76" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G76" s="5">
         <v>42</v>
@@ -3207,13 +3214,13 @@
         <v>4</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F77" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G77" s="5">
         <v>48</v>
@@ -3230,13 +3237,13 @@
         <v>4</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G78" s="5">
         <v>60</v>
@@ -3253,13 +3260,13 @@
         <v>4</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G79" s="5">
         <v>104</v>
@@ -3276,13 +3283,13 @@
         <v>4</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F80" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G80" s="5">
         <v>225</v>
@@ -3299,13 +3306,13 @@
         <v>4</v>
       </c>
       <c r="D81" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E81" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F81" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G81" s="5">
         <v>2</v>
@@ -3322,13 +3329,13 @@
         <v>4</v>
       </c>
       <c r="D82" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E82" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F82" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G82" s="5">
         <v>60</v>
@@ -3345,13 +3352,13 @@
         <v>4</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E83" s="5" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F83" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G83" s="5">
         <v>9</v>
@@ -3368,13 +3375,13 @@
         <v>4</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E84" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G84" s="5">
         <v>536</v>
@@ -3391,13 +3398,13 @@
         <v>4</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E85" s="5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F85" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G85" s="5">
         <v>42</v>
@@ -3414,13 +3421,13 @@
         <v>4</v>
       </c>
       <c r="D86" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E86" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F86" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G86" s="5">
         <v>38</v>
@@ -3437,13 +3444,13 @@
         <v>4</v>
       </c>
       <c r="D87" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E87" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F87" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G87" s="5">
         <v>130</v>
@@ -3464,13 +3471,13 @@
         <v>1</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G88" s="2">
         <v>32</v>
@@ -3487,13 +3494,13 @@
         <v>1</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G89" s="2">
         <v>30</v>
@@ -3510,13 +3517,13 @@
         <v>1</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G90" s="2">
         <v>100</v>
@@ -3533,13 +3540,13 @@
         <v>1</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G91" s="2">
         <v>540</v>
@@ -3556,13 +3563,13 @@
         <v>1</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G92" s="2">
         <v>36</v>
@@ -3579,13 +3586,13 @@
         <v>1</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G93" s="2">
         <v>315</v>
@@ -3602,13 +3609,13 @@
         <v>1</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G94" s="2">
         <v>6</v>
@@ -3629,13 +3636,13 @@
         <v>2</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F95" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G95" s="3">
         <v>20</v>
@@ -3652,13 +3659,13 @@
         <v>2</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F96" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G96" s="3">
         <v>102</v>
@@ -3675,13 +3682,13 @@
         <v>2</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F97" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G97" s="3">
         <v>46</v>
@@ -3702,13 +3709,13 @@
         <v>2</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G98" s="3">
         <v>16</v>
@@ -3729,13 +3736,13 @@
         <v>2</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G99" s="3">
         <v>437.5</v>
@@ -3756,13 +3763,13 @@
         <v>2</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F100" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G100" s="3">
         <v>337.75</v>
@@ -3783,13 +3790,13 @@
         <v>2</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F101" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G101" s="3">
         <v>124</v>
@@ -3810,13 +3817,13 @@
         <v>2</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F102" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G102" s="3">
         <v>706</v>
@@ -3837,13 +3844,13 @@
         <v>2</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F103" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G103" s="3">
         <v>220</v>
@@ -3864,13 +3871,13 @@
         <v>2</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E104" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F104" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G104" s="3">
         <v>300</v>
@@ -3891,13 +3898,13 @@
         <v>2</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E105" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F105" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G105" s="3">
         <v>56</v>
@@ -3918,13 +3925,13 @@
         <v>2</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E106" s="3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F106" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G106" s="3">
         <v>195</v>
@@ -3945,13 +3952,13 @@
         <v>2</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E107" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F107" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G107" s="3">
         <v>196</v>
@@ -3972,13 +3979,13 @@
         <v>2</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E108" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F108" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G108" s="3">
         <v>378</v>
@@ -3999,19 +4006,16 @@
         <v>2</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F109" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G109" s="3">
         <v>205</v>
-      </c>
-      <c r="I109" s="1" t="s">
-        <v>125</v>
       </c>
       <c r="O109"/>
       <c r="P109"/>
@@ -4029,19 +4033,16 @@
         <v>2</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E110" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F110" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G110" s="3">
         <v>104</v>
-      </c>
-      <c r="I110" s="1" t="s">
-        <v>125</v>
       </c>
       <c r="O110"/>
       <c r="P110"/>
@@ -4059,19 +4060,16 @@
         <v>2</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E111" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F111" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G111" s="3">
         <v>90</v>
-      </c>
-      <c r="I111" s="1" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="112" spans="1:18" x14ac:dyDescent="0.25">
@@ -4085,22 +4083,19 @@
         <v>2</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E112" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F112" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G112" s="3">
         <v>9</v>
       </c>
-      <c r="I112" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="3">
         <v>112</v>
       </c>
@@ -4111,22 +4106,19 @@
         <v>2</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F113" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G113" s="3">
         <v>37</v>
       </c>
-      <c r="I113" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="3">
         <v>113</v>
       </c>
@@ -4137,22 +4129,19 @@
         <v>2</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E114" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F114" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G114" s="3">
         <v>120</v>
       </c>
-      <c r="I114" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="3">
         <v>114</v>
       </c>
@@ -4163,19 +4152,19 @@
         <v>2</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E115" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F115" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G115" s="3">
         <v>306</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="3">
         <v>115</v>
       </c>
@@ -4186,16 +4175,154 @@
         <v>2</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E116" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F116" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G116" s="3">
         <v>156</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A117" s="3">
+        <v>116</v>
+      </c>
+      <c r="B117" s="3">
+        <v>2022</v>
+      </c>
+      <c r="C117" s="3">
+        <v>2</v>
+      </c>
+      <c r="D117" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="E117" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="F117" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G117" s="3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A118" s="3">
+        <v>117</v>
+      </c>
+      <c r="B118" s="3">
+        <v>2022</v>
+      </c>
+      <c r="C118" s="3">
+        <v>2</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="E118" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="F118" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G118" s="3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A119" s="3">
+        <v>118</v>
+      </c>
+      <c r="B119" s="3">
+        <v>2022</v>
+      </c>
+      <c r="C119" s="3">
+        <v>2</v>
+      </c>
+      <c r="D119" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="E119" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="F119" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G119" s="3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A120" s="3">
+        <v>119</v>
+      </c>
+      <c r="B120" s="3">
+        <v>2022</v>
+      </c>
+      <c r="C120" s="3">
+        <v>2</v>
+      </c>
+      <c r="D120" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="E120" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="F120" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G120" s="3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A121" s="3">
+        <v>120</v>
+      </c>
+      <c r="B121" s="3">
+        <v>2022</v>
+      </c>
+      <c r="C121" s="3">
+        <v>2</v>
+      </c>
+      <c r="D121" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="E121" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="F121" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G121" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A122" s="3">
+        <v>121</v>
+      </c>
+      <c r="B122" s="3">
+        <v>2022</v>
+      </c>
+      <c r="C122" s="3">
+        <v>2</v>
+      </c>
+      <c r="D122" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="E122" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F122" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G122" s="3">
+        <v>430.9</v>
       </c>
     </row>
   </sheetData>
@@ -4209,8 +4336,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4225,18 +4352,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="9"/>
+      <c r="A1" s="11"/>
       <c r="B1" s="11" t="s">
-        <v>4</v>
+        <v>104</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>105</v>
+        <v>13</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F1" s="11" t="s">
         <v>17</v>
@@ -4248,10 +4375,10 @@
         <v>19</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="K1" s="11" t="s">
         <v>26</v>
@@ -4259,252 +4386,264 @@
       <c r="L1" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="M1" s="11" t="s">
-        <v>28</v>
+      <c r="M1" s="14" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="8">
+        <v>1433</v>
+      </c>
+      <c r="C2" s="8">
+        <v>1513</v>
+      </c>
+      <c r="D2" s="8">
+        <v>1565</v>
+      </c>
+      <c r="E2" s="8">
+        <v>1590</v>
+      </c>
+      <c r="F2" s="8">
+        <v>1596</v>
+      </c>
+      <c r="G2" s="8">
+        <v>1521</v>
+      </c>
+      <c r="H2" s="8">
+        <v>1584</v>
+      </c>
+      <c r="I2" s="8">
+        <v>1600</v>
+      </c>
+      <c r="J2" s="8">
+        <v>1482</v>
+      </c>
+      <c r="K2" s="8">
+        <v>1516</v>
+      </c>
+      <c r="L2" s="8">
+        <v>1645</v>
+      </c>
+      <c r="M2" s="15">
+        <v>1682</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="8">
-        <v>1433</v>
-      </c>
-      <c r="D2" s="8">
-        <v>1513</v>
-      </c>
-      <c r="E2" s="8">
-        <v>1565</v>
-      </c>
-      <c r="F2" s="8">
-        <v>1590</v>
-      </c>
-      <c r="G2" s="8">
-        <v>1596</v>
-      </c>
-      <c r="H2" s="8">
-        <v>1521</v>
-      </c>
-      <c r="I2" s="8">
-        <v>1584</v>
-      </c>
-      <c r="J2" s="8">
-        <v>1600</v>
-      </c>
-      <c r="K2" s="8">
-        <v>1482</v>
-      </c>
-      <c r="L2" s="8">
-        <v>1516</v>
-      </c>
-      <c r="M2" s="8">
-        <v>1645</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="8">
+        <v>652</v>
+      </c>
+      <c r="C3" s="8">
+        <v>651</v>
+      </c>
+      <c r="D3" s="8">
+        <v>670</v>
+      </c>
+      <c r="E3" s="8">
+        <v>679</v>
+      </c>
+      <c r="F3" s="8">
+        <v>673</v>
+      </c>
+      <c r="G3" s="8">
+        <v>625</v>
+      </c>
+      <c r="H3" s="8">
+        <v>643</v>
+      </c>
+      <c r="I3" s="8">
+        <v>641</v>
+      </c>
+      <c r="J3" s="8">
+        <v>586</v>
+      </c>
+      <c r="K3" s="8">
+        <v>602</v>
+      </c>
+      <c r="L3" s="8">
+        <v>638</v>
+      </c>
+      <c r="M3" s="15">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="8">
-        <v>652</v>
-      </c>
-      <c r="D3" s="8">
-        <v>651</v>
-      </c>
-      <c r="E3" s="8">
-        <v>670</v>
-      </c>
-      <c r="F3" s="8">
-        <v>679</v>
-      </c>
-      <c r="G3" s="8">
-        <v>673</v>
-      </c>
-      <c r="H3" s="8">
-        <v>625</v>
-      </c>
-      <c r="I3" s="8">
-        <v>643</v>
-      </c>
-      <c r="J3" s="8">
-        <v>641</v>
-      </c>
-      <c r="K3" s="8">
-        <v>586</v>
-      </c>
-      <c r="L3" s="8">
-        <v>602</v>
-      </c>
-      <c r="M3" s="8">
-        <v>638</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="8">
+        <v>10</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8">
+        <v>6</v>
+      </c>
+      <c r="E4" s="8">
+        <v>0</v>
+      </c>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8">
         <v>8</v>
       </c>
-      <c r="C4" s="8">
+      <c r="H4" s="8">
+        <v>5</v>
+      </c>
+      <c r="I4" s="8">
+        <v>54</v>
+      </c>
+      <c r="J4" s="8">
+        <v>0</v>
+      </c>
+      <c r="K4" s="8">
+        <v>3</v>
+      </c>
+      <c r="L4" s="8">
+        <v>0</v>
+      </c>
+      <c r="M4" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="8">
+        <v>1163</v>
+      </c>
+      <c r="C5" s="8">
+        <v>1170</v>
+      </c>
+      <c r="D5" s="8">
+        <v>1275</v>
+      </c>
+      <c r="E5" s="8">
+        <v>1276</v>
+      </c>
+      <c r="F5" s="8">
+        <v>1257</v>
+      </c>
+      <c r="G5" s="8">
+        <v>1284</v>
+      </c>
+      <c r="H5" s="8">
+        <v>1302</v>
+      </c>
+      <c r="I5" s="8">
+        <v>1284</v>
+      </c>
+      <c r="J5" s="8">
+        <v>1439</v>
+      </c>
+      <c r="K5" s="8">
+        <v>1466</v>
+      </c>
+      <c r="L5" s="8">
+        <v>1606</v>
+      </c>
+      <c r="M5" s="15">
+        <v>1637</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8">
         <v>10</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8">
-        <v>6</v>
-      </c>
-      <c r="F4" s="8">
-        <v>0</v>
-      </c>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8">
-        <v>8</v>
-      </c>
-      <c r="I4" s="8">
-        <v>5</v>
-      </c>
-      <c r="J4" s="8">
-        <v>54</v>
-      </c>
-      <c r="K4" s="8">
-        <v>0</v>
-      </c>
-      <c r="L4" s="8">
-        <v>3</v>
-      </c>
-      <c r="M4" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="8">
-        <v>1163</v>
-      </c>
-      <c r="D5" s="8">
-        <v>1170</v>
-      </c>
-      <c r="E5" s="8">
-        <v>1275</v>
-      </c>
-      <c r="F5" s="8">
-        <v>1276</v>
-      </c>
-      <c r="G5" s="8">
-        <v>1257</v>
-      </c>
-      <c r="H5" s="8">
-        <v>1284</v>
-      </c>
-      <c r="I5" s="8">
-        <v>1302</v>
-      </c>
-      <c r="J5" s="8">
-        <v>1284</v>
-      </c>
-      <c r="K5" s="8">
-        <v>1439</v>
-      </c>
-      <c r="L5" s="8">
-        <v>1466</v>
-      </c>
-      <c r="M5" s="8">
-        <v>1606</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
       <c r="E6" s="8">
         <v>10</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8">
+        <v>50</v>
+      </c>
+      <c r="I6" s="8">
+        <v>20</v>
+      </c>
+      <c r="J6" s="8">
+        <v>0</v>
+      </c>
+      <c r="K6" s="8">
+        <v>50</v>
+      </c>
+      <c r="L6" s="8">
+        <v>0</v>
+      </c>
+      <c r="M6" s="15">
         <v>10</v>
       </c>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8">
-        <v>50</v>
-      </c>
-      <c r="J6" s="8">
-        <v>20</v>
-      </c>
-      <c r="K6" s="8">
-        <v>0</v>
-      </c>
-      <c r="L6" s="8">
-        <v>50</v>
-      </c>
-      <c r="M6" s="8">
-        <v>0</v>
-      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="12" t="s">
-        <v>10</v>
+      <c r="A7" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="8">
+        <v>200</v>
       </c>
       <c r="C7" s="8">
         <v>200</v>
       </c>
       <c r="D7" s="8">
-        <v>200</v>
+        <v>225</v>
       </c>
       <c r="E7" s="8">
         <v>225</v>
       </c>
       <c r="F7" s="8">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="G7" s="8">
-        <v>218</v>
+        <v>192</v>
       </c>
       <c r="H7" s="8">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I7" s="8">
-        <v>191</v>
+        <v>143</v>
       </c>
       <c r="J7" s="8">
-        <v>143</v>
+        <v>120</v>
       </c>
       <c r="K7" s="8">
-        <v>120</v>
+        <v>166</v>
       </c>
       <c r="L7" s="8">
-        <v>166</v>
-      </c>
-      <c r="M7" s="8">
         <v>145</v>
       </c>
+      <c r="M7" s="15">
+        <v>106</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="12" t="s">
-        <v>11</v>
-      </c>
+      <c r="A8" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
+      <c r="F8" s="8">
+        <v>7</v>
+      </c>
       <c r="G8" s="8">
-        <v>7</v>
-      </c>
-      <c r="H8" s="8">
         <v>6</v>
       </c>
-      <c r="I8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8">
+        <v>8</v>
+      </c>
       <c r="J8" s="8">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="K8" s="8">
         <v>0</v>
@@ -4512,108 +4651,111 @@
       <c r="L8" s="8">
         <v>0</v>
       </c>
-      <c r="M8" s="8">
-        <v>0</v>
-      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="12" t="s">
+      <c r="A9" s="12" t="s">
         <v>3</v>
       </c>
+      <c r="B9" s="8">
+        <v>633</v>
+      </c>
       <c r="C9" s="8">
-        <v>633</v>
+        <v>616</v>
       </c>
       <c r="D9" s="8">
-        <v>616</v>
+        <v>620</v>
       </c>
       <c r="E9" s="8">
+        <v>640</v>
+      </c>
+      <c r="F9" s="8">
+        <v>630</v>
+      </c>
+      <c r="G9" s="8">
+        <v>600</v>
+      </c>
+      <c r="H9" s="8">
+        <v>611</v>
+      </c>
+      <c r="I9" s="8">
         <v>620</v>
       </c>
-      <c r="F9" s="8">
-        <v>640</v>
-      </c>
-      <c r="G9" s="8">
-        <v>630</v>
-      </c>
-      <c r="H9" s="8">
-        <v>600</v>
-      </c>
-      <c r="I9" s="8">
-        <v>611</v>
-      </c>
       <c r="J9" s="8">
-        <v>620</v>
+        <v>654</v>
       </c>
       <c r="K9" s="8">
-        <v>654</v>
+        <v>674</v>
       </c>
       <c r="L9" s="8">
-        <v>674</v>
-      </c>
-      <c r="M9" s="8">
         <v>752</v>
       </c>
+      <c r="M9" s="15">
+        <v>794</v>
+      </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="12" t="s">
-        <v>13</v>
+      <c r="A10" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="8">
+        <v>20</v>
       </c>
       <c r="C10" s="8">
         <v>20</v>
       </c>
       <c r="D10" s="8">
-        <v>20</v>
-      </c>
-      <c r="E10" s="8">
         <v>21</v>
       </c>
-      <c r="F10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8">
+        <v>14</v>
+      </c>
       <c r="G10" s="8">
         <v>14</v>
       </c>
       <c r="H10" s="8">
+        <v>17</v>
+      </c>
+      <c r="I10" s="8">
         <v>14</v>
       </c>
-      <c r="I10" s="8">
-        <v>17</v>
-      </c>
       <c r="J10" s="8">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="K10" s="8">
         <v>7</v>
       </c>
       <c r="L10" s="8">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="M10" s="8">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="12" t="s">
-        <v>16</v>
-      </c>
+      <c r="A11" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="8"/>
       <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8">
+      <c r="D11" s="8">
         <v>10</v>
       </c>
-      <c r="F11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8">
+        <v>8</v>
+      </c>
       <c r="G11" s="8">
+        <v>7</v>
+      </c>
+      <c r="H11" s="8">
         <v>8</v>
-      </c>
-      <c r="H11" s="8">
-        <v>7</v>
       </c>
       <c r="I11" s="8">
         <v>8</v>
       </c>
       <c r="J11" s="8">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="K11" s="8">
         <v>3</v>
@@ -4626,21 +4768,23 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="12" t="s">
-        <v>21</v>
-      </c>
+      <c r="A12" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
+      <c r="H12" s="8">
+        <v>10</v>
+      </c>
       <c r="I12" s="8">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J12" s="8">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K12" s="8">
         <v>7</v>
@@ -4653,79 +4797,82 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="12" t="s">
-        <v>25</v>
-      </c>
+      <c r="A13" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="8"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
+      <c r="I13" s="8">
+        <v>109</v>
+      </c>
       <c r="J13" s="8">
-        <v>109</v>
+        <v>145</v>
       </c>
       <c r="K13" s="8">
-        <v>145</v>
+        <v>178</v>
       </c>
       <c r="L13" s="8">
         <v>178</v>
       </c>
-      <c r="M13" s="8">
-        <v>178</v>
+      <c r="M13" s="15">
+        <v>193</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="12" t="s">
-        <v>24</v>
-      </c>
+      <c r="A14" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="8"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
+      <c r="I14" s="8">
+        <v>66</v>
+      </c>
       <c r="J14" s="8">
-        <v>66</v>
-      </c>
-      <c r="K14" s="8">
         <v>0</v>
       </c>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8">
+      <c r="K14" s="8"/>
+      <c r="L14" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="C15" s="8"/>
+      <c r="A15" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8">
+        <v>123</v>
+      </c>
       <c r="D15" s="8">
         <v>123</v>
       </c>
-      <c r="E15" s="8">
-        <v>123</v>
-      </c>
+      <c r="E15" s="8"/>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
       <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8">
+      <c r="L15" s="8">
         <v>148</v>
       </c>
+      <c r="M15">
+        <v>148</v>
+      </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="12"/>
+      <c r="A16" s="12"/>
+      <c r="B16" s="8"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
@@ -4736,11 +4883,10 @@
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
       <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
-      <c r="B17" s="12"/>
+      <c r="A17" s="12"/>
+      <c r="B17" s="8"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
@@ -4751,25 +4897,26 @@
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
       <c r="L17" s="8"/>
-      <c r="M17" s="8"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="12" t="s">
+      <c r="A18" s="12" t="s">
         <v>0</v>
       </c>
+      <c r="B18" s="8">
+        <v>73</v>
+      </c>
       <c r="C18" s="8">
-        <v>73</v>
+        <v>95</v>
       </c>
       <c r="D18" s="8">
-        <v>95</v>
-      </c>
-      <c r="E18" s="8">
         <v>70</v>
       </c>
-      <c r="F18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8">
+        <v>50</v>
+      </c>
       <c r="G18" s="8">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="H18" s="8">
         <v>45</v>
@@ -4777,78 +4924,73 @@
       <c r="I18" s="8">
         <v>45</v>
       </c>
-      <c r="J18" s="8">
-        <v>45</v>
-      </c>
+      <c r="J18" s="8"/>
       <c r="K18" s="8"/>
       <c r="L18" s="8"/>
-      <c r="M18" s="8"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
-      <c r="B19" s="12" t="s">
-        <v>12</v>
+      <c r="A19" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="8">
+        <v>74</v>
       </c>
       <c r="C19" s="8">
-        <v>74</v>
+        <v>25</v>
       </c>
       <c r="D19" s="8">
-        <v>25</v>
-      </c>
-      <c r="E19" s="8">
         <v>15</v>
       </c>
-      <c r="F19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8">
+        <v>14</v>
+      </c>
       <c r="G19" s="8">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="H19" s="8">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="I19" s="8">
-        <v>20</v>
-      </c>
-      <c r="J19" s="8">
         <v>10</v>
       </c>
+      <c r="J19" s="8"/>
       <c r="K19" s="8"/>
       <c r="L19" s="8"/>
-      <c r="M19" s="8"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
-      <c r="B20" s="12" t="s">
+      <c r="A20" s="12" t="s">
         <v>1</v>
       </c>
+      <c r="B20" s="8">
+        <v>50</v>
+      </c>
       <c r="C20" s="8">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="D20" s="8">
-        <v>58</v>
-      </c>
-      <c r="E20" s="8">
         <v>90</v>
       </c>
-      <c r="F20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8">
+        <v>131</v>
+      </c>
       <c r="G20" s="8">
-        <v>131</v>
+        <v>63</v>
       </c>
       <c r="H20" s="8">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="I20" s="8">
-        <v>77</v>
-      </c>
-      <c r="J20" s="8">
         <v>28</v>
       </c>
+      <c r="J20" s="8"/>
       <c r="K20" s="8"/>
       <c r="L20" s="8"/>
-      <c r="M20" s="8"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
-      <c r="B21" s="12"/>
+      <c r="A21" s="12"/>
+      <c r="B21" s="8"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
@@ -4859,11 +5001,10 @@
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
       <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
-      <c r="B22" s="12"/>
+      <c r="A22" s="12"/>
+      <c r="B22" s="8"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
@@ -4874,43 +5015,62 @@
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
       <c r="L22" s="8"/>
-      <c r="M22" s="8"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
-      <c r="B23" s="12" t="s">
-        <v>22</v>
-      </c>
+      <c r="A23" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="8"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8">
+      <c r="H23" s="8">
         <v>1000</v>
       </c>
-      <c r="J23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8">
+        <v>1059</v>
+      </c>
       <c r="K23" s="8">
         <v>1059</v>
       </c>
       <c r="L23" s="8">
-        <v>1059</v>
+        <v>1082</v>
       </c>
       <c r="M23" s="8">
         <v>1082</v>
       </c>
     </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M24">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M25">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M26">
+        <v>160</v>
+      </c>
+    </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="B27" s="16"/>
+      <c r="A27" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="B27" s="17"/>
       <c r="C27" s="10"/>
+      <c r="M27">
+        <v>80</v>
+      </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B28" s="7">
         <v>23067</v>
@@ -4957,8 +5117,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A2:A23"/>
+  <mergeCells count="1">
     <mergeCell ref="A27:B27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4983,23 +5142,23 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F1" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="G1" s="9" t="s">
         <v>114</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -5007,7 +5166,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="8">
@@ -5024,7 +5183,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8">
@@ -5041,7 +5200,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="8">
@@ -5058,7 +5217,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="8">
@@ -5074,7 +5233,7 @@
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
@@ -5087,7 +5246,7 @@
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
@@ -5097,10 +5256,10 @@
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>117</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>118</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>

</xml_diff>